<commit_message>
Update Sample form - Display iframe.xlsx
</commit_message>
<xml_diff>
--- a/extras/sample-form/Sample form - Display iframe.xlsx
+++ b/extras/sample-form/Sample form - Display iframe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\display-graph\extras\sample-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EBD445-B4CF-4967-9974-5BC91E23688C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0A6EAC-7262-4A9F-BD23-44B1C142D71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="14385" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="379">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2574,10 +2574,6 @@
     <t/>
   </si>
   <si>
-    <t xml:space="preserve">Welcome to this sample form for the display-iframe field plug-in. The plug-in allows you to display a web-published graph from Google sheets, or other web content in an iframe, in your form. This demo displays graphs from Google Sheets.&lt;br&gt; 
-You can learn about &lt;a href="https://support.google.com/docs/answer/1047436?co=GENIE.Platform%3DDesktop&amp;hl=en" target="_blank"&gt;how to publish a chart here. &lt;/a&gt; </t>
-  </si>
-  <si>
     <t>display_pie_chart</t>
   </si>
   <si>
@@ -2631,6 +2627,18 @@
   </si>
   <si>
     <t>item-at('|',plug-in-metadata(${display_pie_chart}), 1)</t>
+  </si>
+  <si>
+    <t>intro</t>
+  </si>
+  <si>
+    <t>Welcome to this sample form for the display-iframe field plug-in. The plug-in allows you to display a web-published graph from Google sheets, or other web content in an iframe, in your form. This demo displays graphs from Google Sheets.&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+The following resources are useful in understanding the sample form:&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="https://github.com/surveycto/display-iframe/blob/master/README.md" target="_blank"&gt;Plug-in overview&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://docs.google.com/spreadsheets/d/1celfPEyKUThteeWtJtb0JptUmzX7QNCPuwBXlcWJLTI/edit#gid=883786841" target="_blank"&gt;Sample data file&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://support.google.com/docs/answer/1047436?co=GENIE.Platform%3DDesktop&amp;hl=en" target="_blank"&gt;How to publish a chart to the web in Google Sheets&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -4764,7 +4772,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13:D14"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -4963,15 +4971,18 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:23" ht="218.4">
+    <row r="12" spans="1:23" ht="409.5">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>359</v>
+        <v>378</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>377</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -4981,16 +4992,16 @@
         <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -4998,16 +5009,16 @@
         <v>96</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>363</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -5015,13 +5026,13 @@
         <v>148</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>366</v>
-      </c>
       <c r="N15" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -5029,13 +5040,13 @@
         <v>148</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>368</v>
-      </c>
       <c r="N16" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="62.4">
@@ -5043,10 +5054,10 @@
         <v>42</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>370</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -5333,14 +5344,14 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>372</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>373</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2010080808</v>
+        <v>2010081755</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>

</xml_diff>